<commit_message>
Doan day file bieu mau
</commit_message>
<xml_diff>
--- a/Document/2.Design/Template/Bieu_mau_hang_hoa.xlsx
+++ b/Document/2.Design/Template/Bieu_mau_hang_hoa.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WMS\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WMS\temp\file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31917334-5D4A-4493-949E-89DDE1FD4ADD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8145"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HangHoa" sheetId="1" r:id="rId1"/>
+    <sheet name="DonVi" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,40 +26,201 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Mã hàng(*)</t>
-  </si>
-  <si>
-    <t>Tên hàng(*)</t>
-  </si>
-  <si>
-    <t>Đơn vị tính</t>
-  </si>
-  <si>
-    <t>QL Serial(*)</t>
-  </si>
-  <si>
-    <t>Trạng thái(*)</t>
-  </si>
-  <si>
     <t>Giá nhập</t>
   </si>
   <si>
     <t>Giá xuất</t>
   </si>
   <si>
-    <t>Nhóm hàng hóa(*)</t>
+    <t>Bao</t>
+  </si>
+  <si>
+    <t>Bình</t>
+  </si>
+  <si>
+    <t>Chiếc</t>
+  </si>
+  <si>
+    <t>Cuốn</t>
+  </si>
+  <si>
+    <t>Cuộn</t>
+  </si>
+  <si>
+    <t>Cái</t>
+  </si>
+  <si>
+    <t>Cây</t>
+  </si>
+  <si>
+    <t>Gói</t>
+  </si>
+  <si>
+    <t>Hộp</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>Lít</t>
+  </si>
+  <si>
+    <t>Lọ</t>
+  </si>
+  <si>
+    <t>Mét</t>
+  </si>
+  <si>
+    <t>Tạ</t>
+  </si>
+  <si>
+    <t>Tấn</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>Mã đơn vị tính</t>
+  </si>
+  <si>
+    <t>Tên đơn vị tính</t>
+  </si>
+  <si>
+    <r>
+      <t>Mã hàng</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tên hàng</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mã đơn vị tính</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(Sheet DonVi)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Nhóm hàng hóa</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>QL Serial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(*)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1: Có
+0: Không</t>
+    </r>
+  </si>
+  <si>
+    <t>Trọng lượng (Kg)</t>
+  </si>
+  <si>
+    <t>Cao(cm)</t>
+  </si>
+  <si>
+    <t>Rộng(cm)</t>
+  </si>
+  <si>
+    <t>Dài(cm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +230,36 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -112,17 +305,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -434,57 +634,245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" style="5" customWidth="1"/>
+    <col min="9" max="12" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
+      <c r="I1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D873F7-52EF-45C9-A991-9A58CF190C43}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>